<commit_message>
added front end folder
</commit_message>
<xml_diff>
--- a/Project Schedule.xlsx
+++ b/Project Schedule.xlsx
@@ -5,20 +5,20 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Artificial Intelligence\Term I\Capstone Term I - 1003\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38061842-C076-4298-932B-4284D4AA7DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCE356A-BB39-4FC6-AA89-37CF57172BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
+    <sheet name="Project schedule" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BK$16</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
+    <definedName name="prevWBS" localSheetId="0">'Project schedule'!$A1048576</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Project schedule'!$A$1:$BK$16</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project schedule'!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2006-2018 Vertex42 LLC"</definedName>
     <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
@@ -1034,7 +1034,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1113,9 +1113,6 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1136,6 +1133,24 @@
     <xf numFmtId="165" fontId="3" fillId="23" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1146,27 +1161,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="33" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1633,6 +1630,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -1665,16 +1672,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2183,9 +2180,9 @@
   </sheetPr>
   <dimension ref="A1:BY25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S25" sqref="S25"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2217,35 +2214,35 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
     </row>
     <row r="2" spans="1:77" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:77" ht="13.8" x14ac:dyDescent="0.25">
@@ -2275,226 +2272,226 @@
       <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="44">
         <v>44837</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <v>1</v>
       </c>
-      <c r="H4" s="39" t="str">
+      <c r="H4" s="35" t="str">
         <f>"Week "&amp;(H6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="39" t="str">
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="35" t="str">
         <f>"Week "&amp;(O6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="39" t="str">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="35" t="str">
         <f>"Week "&amp;(V6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="41"/>
-      <c r="AC4" s="39" t="str">
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="35" t="str">
         <f>"Week "&amp;(AC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
-      <c r="AI4" s="41"/>
-      <c r="AJ4" s="39" t="str">
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="36"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="35" t="str">
         <f>"Week "&amp;(AJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AK4" s="40"/>
-      <c r="AL4" s="40"/>
-      <c r="AM4" s="40"/>
-      <c r="AN4" s="40"/>
-      <c r="AO4" s="40"/>
-      <c r="AP4" s="41"/>
-      <c r="AQ4" s="39" t="str">
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="36"/>
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="36"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="35" t="str">
         <f>"Week "&amp;(AQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AR4" s="40"/>
-      <c r="AS4" s="40"/>
-      <c r="AT4" s="40"/>
-      <c r="AU4" s="40"/>
-      <c r="AV4" s="40"/>
-      <c r="AW4" s="41"/>
-      <c r="AX4" s="39" t="str">
+      <c r="AR4" s="36"/>
+      <c r="AS4" s="36"/>
+      <c r="AT4" s="36"/>
+      <c r="AU4" s="36"/>
+      <c r="AV4" s="36"/>
+      <c r="AW4" s="37"/>
+      <c r="AX4" s="35" t="str">
         <f>"Week "&amp;(AX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AY4" s="40"/>
-      <c r="AZ4" s="40"/>
-      <c r="BA4" s="40"/>
-      <c r="BB4" s="40"/>
-      <c r="BC4" s="40"/>
-      <c r="BD4" s="41"/>
-      <c r="BE4" s="39" t="str">
+      <c r="AY4" s="36"/>
+      <c r="AZ4" s="36"/>
+      <c r="BA4" s="36"/>
+      <c r="BB4" s="36"/>
+      <c r="BC4" s="36"/>
+      <c r="BD4" s="37"/>
+      <c r="BE4" s="35" t="str">
         <f>"Week "&amp;(BE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BF4" s="40"/>
-      <c r="BG4" s="40"/>
-      <c r="BH4" s="40"/>
-      <c r="BI4" s="40"/>
-      <c r="BJ4" s="40"/>
-      <c r="BK4" s="41"/>
-      <c r="BL4" s="39" t="str">
+      <c r="BF4" s="36"/>
+      <c r="BG4" s="36"/>
+      <c r="BH4" s="36"/>
+      <c r="BI4" s="36"/>
+      <c r="BJ4" s="36"/>
+      <c r="BK4" s="37"/>
+      <c r="BL4" s="35" t="str">
         <f>"Week "&amp;(BL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BM4" s="40"/>
-      <c r="BN4" s="40"/>
-      <c r="BO4" s="40"/>
-      <c r="BP4" s="40"/>
-      <c r="BQ4" s="40"/>
-      <c r="BR4" s="41"/>
-      <c r="BS4" s="39" t="str">
+      <c r="BM4" s="36"/>
+      <c r="BN4" s="36"/>
+      <c r="BO4" s="36"/>
+      <c r="BP4" s="36"/>
+      <c r="BQ4" s="36"/>
+      <c r="BR4" s="37"/>
+      <c r="BS4" s="35" t="str">
         <f>"Week "&amp;(BS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BT4" s="40"/>
-      <c r="BU4" s="40"/>
-      <c r="BV4" s="40"/>
-      <c r="BW4" s="40"/>
-      <c r="BX4" s="40"/>
-      <c r="BY4" s="41"/>
+      <c r="BT4" s="36"/>
+      <c r="BU4" s="36"/>
+      <c r="BV4" s="36"/>
+      <c r="BW4" s="36"/>
+      <c r="BX4" s="36"/>
+      <c r="BY4" s="37"/>
     </row>
     <row r="5" spans="1:77" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="43">
+      <c r="H5" s="38">
         <f>H6</f>
         <v>44837</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="43">
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="38">
         <f>O6</f>
         <v>44844</v>
       </c>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="43">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="38">
         <f>V6</f>
         <v>44851</v>
       </c>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="43">
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="38">
         <f>AC6</f>
         <v>44858</v>
       </c>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="44"/>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="43">
+      <c r="AD5" s="39"/>
+      <c r="AE5" s="39"/>
+      <c r="AF5" s="39"/>
+      <c r="AG5" s="39"/>
+      <c r="AH5" s="39"/>
+      <c r="AI5" s="40"/>
+      <c r="AJ5" s="38">
         <f>AJ6</f>
         <v>44865</v>
       </c>
-      <c r="AK5" s="44"/>
-      <c r="AL5" s="44"/>
-      <c r="AM5" s="44"/>
-      <c r="AN5" s="44"/>
-      <c r="AO5" s="44"/>
-      <c r="AP5" s="45"/>
-      <c r="AQ5" s="43">
+      <c r="AK5" s="39"/>
+      <c r="AL5" s="39"/>
+      <c r="AM5" s="39"/>
+      <c r="AN5" s="39"/>
+      <c r="AO5" s="39"/>
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="38">
         <f>AQ6</f>
         <v>44872</v>
       </c>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="44"/>
-      <c r="AT5" s="44"/>
-      <c r="AU5" s="44"/>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="45"/>
-      <c r="AX5" s="43">
+      <c r="AR5" s="39"/>
+      <c r="AS5" s="39"/>
+      <c r="AT5" s="39"/>
+      <c r="AU5" s="39"/>
+      <c r="AV5" s="39"/>
+      <c r="AW5" s="40"/>
+      <c r="AX5" s="38">
         <f>AX6</f>
         <v>44879</v>
       </c>
-      <c r="AY5" s="44"/>
-      <c r="AZ5" s="44"/>
-      <c r="BA5" s="44"/>
-      <c r="BB5" s="44"/>
-      <c r="BC5" s="44"/>
-      <c r="BD5" s="45"/>
-      <c r="BE5" s="43">
+      <c r="AY5" s="39"/>
+      <c r="AZ5" s="39"/>
+      <c r="BA5" s="39"/>
+      <c r="BB5" s="39"/>
+      <c r="BC5" s="39"/>
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="38">
         <f>BE6</f>
         <v>44886</v>
       </c>
-      <c r="BF5" s="44"/>
-      <c r="BG5" s="44"/>
-      <c r="BH5" s="44"/>
-      <c r="BI5" s="44"/>
-      <c r="BJ5" s="44"/>
-      <c r="BK5" s="45"/>
-      <c r="BL5" s="43">
+      <c r="BF5" s="39"/>
+      <c r="BG5" s="39"/>
+      <c r="BH5" s="39"/>
+      <c r="BI5" s="39"/>
+      <c r="BJ5" s="39"/>
+      <c r="BK5" s="40"/>
+      <c r="BL5" s="38">
         <f>BL6</f>
         <v>44893</v>
       </c>
-      <c r="BM5" s="44"/>
-      <c r="BN5" s="44"/>
-      <c r="BO5" s="44"/>
-      <c r="BP5" s="44"/>
-      <c r="BQ5" s="44"/>
-      <c r="BR5" s="45"/>
-      <c r="BS5" s="43">
+      <c r="BM5" s="39"/>
+      <c r="BN5" s="39"/>
+      <c r="BO5" s="39"/>
+      <c r="BP5" s="39"/>
+      <c r="BQ5" s="39"/>
+      <c r="BR5" s="40"/>
+      <c r="BS5" s="38">
         <f>BS6</f>
         <v>44900</v>
       </c>
-      <c r="BT5" s="44"/>
-      <c r="BU5" s="44"/>
-      <c r="BV5" s="44"/>
-      <c r="BW5" s="44"/>
-      <c r="BX5" s="44"/>
-      <c r="BY5" s="45"/>
+      <c r="BT5" s="39"/>
+      <c r="BU5" s="39"/>
+      <c r="BV5" s="39"/>
+      <c r="BW5" s="39"/>
+      <c r="BX5" s="39"/>
+      <c r="BY5" s="40"/>
     </row>
     <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
@@ -2544,7 +2541,7 @@
         <f t="shared" si="0"/>
         <v>44846</v>
       </c>
-      <c r="R6" s="35">
+      <c r="R6" s="34">
         <f t="shared" si="0"/>
         <v>44847</v>
       </c>
@@ -2789,10 +2786,10 @@
       <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="20" t="s">
         <v>5</v>
       </c>
@@ -3094,10 +3091,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="27"/>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>44837</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>44843</v>
       </c>
       <c r="G8" s="12">
@@ -3168,10 +3165,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="27"/>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <v>44844</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>44850</v>
       </c>
       <c r="G9" s="12">
@@ -3242,10 +3239,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="27"/>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>44851</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <v>44857</v>
       </c>
       <c r="G10" s="12">
@@ -3316,10 +3313,10 @@
         <v>14</v>
       </c>
       <c r="D11" s="27"/>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>44858</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="32">
         <v>44864</v>
       </c>
       <c r="G11" s="12">
@@ -3386,14 +3383,14 @@
       <c r="A12" s="10">
         <v>5</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>44865</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <v>44871</v>
       </c>
       <c r="G12" s="12">
@@ -3460,14 +3457,14 @@
       <c r="A13" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <v>44872</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <v>44878</v>
       </c>
       <c r="G13" s="12">
@@ -3538,10 +3535,10 @@
         <v>17</v>
       </c>
       <c r="D14" s="27"/>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <v>44879</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <v>44885</v>
       </c>
       <c r="G14" s="12">
@@ -3612,10 +3609,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>44886</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <v>44892</v>
       </c>
       <c r="G15" s="12">
@@ -3686,10 +3683,10 @@
         <v>11</v>
       </c>
       <c r="D16" s="27"/>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <v>44893</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="32">
         <v>44899</v>
       </c>
       <c r="G16" s="12">
@@ -3764,13 +3761,13 @@
       <c r="A17" s="10">
         <v>10</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="31">
         <v>44900</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <v>44906</v>
       </c>
       <c r="G17" s="12">
@@ -3788,11 +3785,21 @@
       <c r="E20" s="5"/>
     </row>
     <row r="25" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="X25" s="31"/>
+      <c r="X25" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="24">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="H1:AB1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="V5:AB5"/>
     <mergeCell ref="BL4:BR4"/>
     <mergeCell ref="BL5:BR5"/>
     <mergeCell ref="BS4:BY4"/>
@@ -3807,16 +3814,6 @@
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AX4:BD4"/>
     <mergeCell ref="AX5:BD5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="H1:AB1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="O5:U5"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="V5:AB5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G8:G17">
@@ -3839,27 +3836,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:BK16">
-    <cfRule type="expression" dxfId="47" priority="57">
+    <cfRule type="expression" dxfId="51" priority="57">
       <formula>H$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL6:BR7">
-    <cfRule type="expression" dxfId="51" priority="49">
+    <cfRule type="expression" dxfId="50" priority="49">
       <formula>BL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL6:BR7">
-    <cfRule type="expression" dxfId="50" priority="48">
+    <cfRule type="expression" dxfId="49" priority="48">
       <formula>BL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS6:BY7">
-    <cfRule type="expression" dxfId="49" priority="47">
+    <cfRule type="expression" dxfId="48" priority="47">
       <formula>BS$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS6:BY7">
-    <cfRule type="expression" dxfId="48" priority="46">
+    <cfRule type="expression" dxfId="47" priority="46">
       <formula>BS$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4070,7 +4067,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="G4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
-  <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>